<commit_message>
final comments and stuff
</commit_message>
<xml_diff>
--- a/output_base_C1.xlsx
+++ b/output_base_C1.xlsx
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>-5.775894217945515</v>
+        <v>-5.775894217945511</v>
       </c>
     </row>
     <row r="3">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>-11.84863865381283</v>
+        <v>-11.84863865381282</v>
       </c>
     </row>
     <row r="4">
@@ -528,7 +528,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>-8.347063628969877</v>
+        <v>-8.347063628969869</v>
       </c>
     </row>
     <row r="5">
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>-7.187755565451909</v>
+        <v>-7.187755565451902</v>
       </c>
     </row>
     <row r="6">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1.023313014643866</v>
+        <v>1.023313014643867</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>-9.709173348916114</v>
+        <v>-9.709173348916099</v>
       </c>
     </row>
     <row r="7">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.9900031935390051</v>
+        <v>0.9900031935390052</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>-12.4463081887844</v>
+        <v>-12.44630818878438</v>
       </c>
     </row>
     <row r="8">
@@ -624,7 +624,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.9872456593521747</v>
+        <v>0.9872456593521749</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>-12.28545184886834</v>
+        <v>-12.28545184886832</v>
       </c>
     </row>
     <row r="9">
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>-11.17453330640496</v>
+        <v>-11.17453330640495</v>
       </c>
     </row>
     <row r="10">
@@ -684,7 +684,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>-8.587422827861516</v>
+        <v>-8.587422827861504</v>
       </c>
     </row>
     <row r="11">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>-9.918665823988313</v>
+        <v>-9.918665823988295</v>
       </c>
     </row>
     <row r="12">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>-11.04176533061711</v>
+        <v>-11.04176533061709</v>
       </c>
     </row>
   </sheetData>
@@ -773,7 +773,7 @@
         </is>
       </c>
       <c r="D1" t="n">
-        <v>147.2690568675017</v>
+        <v>147.2690568675015</v>
       </c>
       <c r="E1" t="inlineStr">
         <is>
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-61.19674081294561</v>
+        <v>-61.19674081294559</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -851,7 +851,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>27.80384811446033</v>
+        <v>27.80384811446019</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -859,7 +859,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>11.41096661387313</v>
+        <v>11.41096661387309</v>
       </c>
     </row>
     <row r="5">
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>12.10142909103979</v>
+        <v>12.10142909103982</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>18.37846729346686</v>
+        <v>18.37846729346677</v>
       </c>
     </row>
     <row r="6">
@@ -903,7 +903,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-57.81266439111602</v>
+        <v>-57.81266439111604</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -929,7 +929,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-7.578890096896829</v>
+        <v>-7.57889009689687</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>-1.573770468329716</v>
+        <v>-1.573770468329805</v>
       </c>
     </row>
     <row r="8">
@@ -955,7 +955,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>-13.50074925494904</v>
+        <v>-13.50074925494895</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -963,7 +963,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>-8.496484856617936</v>
+        <v>-8.496484856617403</v>
       </c>
     </row>
     <row r="9">
@@ -1007,7 +1007,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-8.999514683423993</v>
+        <v>-8.999514683423882</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1015,7 +1015,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>-5.799533485727437</v>
+        <v>-5.799533485727348</v>
       </c>
     </row>
     <row r="11">
@@ -1041,7 +1041,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>-2.098268090431432</v>
+        <v>-2.098268090431255</v>
       </c>
     </row>
     <row r="12">
@@ -1059,7 +1059,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>-13.49802226177657</v>
+        <v>-13.49802226177665</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1067,7 +1067,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>-5.798933322942545</v>
+        <v>-5.798933322942901</v>
       </c>
     </row>
   </sheetData>
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="F1" t="n">
-        <v>-188.6013384905723</v>
+        <v>-188.6013384905724</v>
       </c>
       <c r="G1" t="inlineStr">
         <is>
@@ -1154,7 +1154,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>-52.81192854638089</v>
+        <v>-52.81192854638096</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -1196,7 +1196,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>-65.73042401196419</v>
+        <v>-65.73042401196423</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -1406,7 +1406,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>13.07347704874359</v>
+        <v>13.07347704874356</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -1448,7 +1448,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>18.41296269444663</v>
+        <v>18.41296269444659</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>-418.1393241255436</v>
+        <v>-418.1393241255437</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>-189.3029415965889</v>
+        <v>-189.302941596589</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1498,7 +1498,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>-423.9790007258065</v>
+        <v>-423.9790007258067</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1506,7 +1506,7 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>464.3207907832418</v>
+        <v>464.320790783242</v>
       </c>
     </row>
     <row r="11">
@@ -1540,7 +1540,7 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>-341.1940832403852</v>
+        <v>-341.1940832403853</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1548,7 +1548,7 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>382.2023799941176</v>
+        <v>382.2023799941177</v>
       </c>
     </row>
     <row r="12">
@@ -1616,7 +1616,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>-384.21981044098</v>
+        <v>-384.2198104409802</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>1082.496208887254</v>
+        <v>1082.496208887255</v>
       </c>
     </row>
     <row r="14">
@@ -1658,7 +1658,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>-154.2164605377792</v>
+        <v>-154.2164605377793</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1666,7 +1666,7 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>-308.184567431635</v>
+        <v>-308.1845674316351</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1674,7 +1674,7 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>344.6163726578068</v>
+        <v>344.6163726578069</v>
       </c>
     </row>
     <row r="15">
@@ -1700,7 +1700,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>-194.1041375817383</v>
+        <v>-194.1041375817384</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1708,7 +1708,7 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>-431.0456545466046</v>
+        <v>-431.0456545466049</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         </is>
       </c>
       <c r="J15" t="n">
-        <v>472.7332995779557</v>
+        <v>472.7332995779559</v>
       </c>
     </row>
     <row r="16">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>-264.5731737406652</v>
+        <v>-264.5731737406653</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -2469,7 +2469,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.05812461064888728</v>
+        <v>0.0581246106488864</v>
       </c>
       <c r="E2" t="n">
         <v>6</v>
@@ -2480,13 +2480,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0002110990310317112</v>
+        <v>0.0002110990310312949</v>
       </c>
       <c r="C3" t="n">
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0002622953167028402</v>
+        <v>0.0002622953167019521</v>
       </c>
       <c r="E3" t="n">
         <v>6</v>

</xml_diff>